<commit_message>
Updated name of field plug-in in sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/scto-twilio-dialer-example.xlsx
+++ b/extras/sample-form/scto-twilio-dialer-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crobert/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Other field plug-in repos/twilio-call/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107C1014-0E26-A248-8094-8D468AB4725F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C2868D-475A-EC49-AFD2-1D80042D0FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="35020" windowHeight="21940" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28720" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2672,9 +2672,6 @@
     <t>pulldata('twilio_access', 'number', 'accessid_key', 1234)</t>
   </si>
   <si>
-    <t>custom-twilio-dialer(fromNumber=${your_number},toNumber=${number_to_call},twilioNumber=${twilio_number},accountSID=${twilio_sid},authToken=${twilio_auth},record=${record_call},displayNumber=${display_number})</t>
-  </si>
-  <si>
     <t>call_attempt</t>
   </si>
   <si>
@@ -2724,6 +2721,9 @@
   </si>
   <si>
     <t>Must begin with country code (like +1 for U.S.)</t>
+  </si>
+  <si>
+    <t>custom-twilio-call(fromNumber=${your_number},toNumber=${number_to_call},twilioNumber=${twilio_number},accountSID=${twilio_sid},authToken=${twilio_auth},record=${record_call},displayNumber=${display_number})</t>
   </si>
 </sst>
 </file>
@@ -4877,7 +4877,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5223,7 +5223,7 @@
         <v>377</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E14" t="str">
         <f>"+1"</f>
@@ -5301,10 +5301,10 @@
         <v>154</v>
       </c>
       <c r="B18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>359</v>
@@ -5327,7 +5327,7 @@
         <v>381</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="K19" t="s">
         <v>374</v>
@@ -5341,7 +5341,7 @@
         <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>359</v>
@@ -5353,7 +5353,7 @@
         <v>359</v>
       </c>
       <c r="N20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -5361,7 +5361,7 @@
         <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>359</v>
@@ -5373,7 +5373,7 @@
         <v>359</v>
       </c>
       <c r="N21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -5381,10 +5381,10 @@
         <v>139</v>
       </c>
       <c r="B22" t="s">
+        <v>405</v>
+      </c>
+      <c r="N22" t="s">
         <v>406</v>
-      </c>
-      <c r="N22" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -5392,10 +5392,10 @@
         <v>139</v>
       </c>
       <c r="B23" t="s">
+        <v>407</v>
+      </c>
+      <c r="N23" t="s">
         <v>408</v>
-      </c>
-      <c r="N23" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5403,7 +5403,7 @@
         <v>155</v>
       </c>
       <c r="B24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -5411,13 +5411,13 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
+        <v>398</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>399</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="I25" t="s">
         <v>400</v>
-      </c>
-      <c r="I25" t="s">
-        <v>401</v>
       </c>
       <c r="K25" t="s">
         <v>374</v>
@@ -5715,14 +5715,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>410</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>411</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006160940</v>
+        <v>2006191513</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -6314,7 +6314,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>93</v>
       </c>

</xml_diff>